<commit_message>
feat:changed column order of temp book in compliance with DR
</commit_message>
<xml_diff>
--- a/renderer/res/Книга тимчасової відсутності.xlsx
+++ b/renderer/res/Книга тимчасової відсутності.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA36A31-DB97-E841-94B9-E055A156B088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2DFFF-A438-2A4D-8E42-66F61481704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,81 +20,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+  <si>
+    <t>Номер документу (посвідчення, довідка, направлення, тощо)</t>
+  </si>
+  <si>
+    <t>Дата реєстрації документа</t>
+  </si>
+  <si>
+    <t>Військове звання (для наочності)</t>
+  </si>
+  <si>
+    <t>Прізвище та ініціали (для наочності)</t>
+  </si>
+  <si>
+    <t>Ідентифікатор військовослужбовця (відповідно до ідентифікатора в словнику)</t>
+  </si>
   <si>
     <t>Тип відсутності</t>
   </si>
   <si>
-    <t>Ідентифікатор військовослужбовця (відповідно до ідентифікатора в словнику)</t>
-  </si>
-  <si>
-    <t>Військове звання (для наочності)</t>
-  </si>
-  <si>
-    <t>Прізвище та ініціали (для наочності)</t>
-  </si>
-  <si>
     <t>Місце тимчасового перебування</t>
   </si>
   <si>
     <t>Дата вибуття</t>
   </si>
   <si>
+    <t>Дата наказу, яким вибув</t>
+  </si>
+  <si>
+    <t>Номер наказу, яким вибув</t>
+  </si>
+  <si>
+    <t>Термін відсутності</t>
+  </si>
+  <si>
     <t>Очікувана дата повернення</t>
   </si>
   <si>
-    <t>Номер документу (посвідчення, довідка, направлення, тощо)</t>
-  </si>
-  <si>
-    <t>Дата реєстрації документа</t>
+    <t>Реальна дата повернення</t>
+  </si>
+  <si>
+    <t>Дата наказу, яким прибув</t>
+  </si>
+  <si>
+    <t>Номер наказу, яким прибув</t>
   </si>
   <si>
     <t>З продовольчим атестатом (так/ні)</t>
   </si>
   <si>
-    <t>Номер наказу, яким вибув</t>
-  </si>
-  <si>
-    <t>Номер наказу, яким прибув</t>
-  </si>
-  <si>
-    <t>Реальна дата повернення</t>
+    <t>2418</t>
+  </si>
+  <si>
+    <t>04.12.2024</t>
+  </si>
+  <si>
+    <t>старший солдат</t>
+  </si>
+  <si>
+    <t>ГРАБОВА Олена Ігорівна</t>
   </si>
   <si>
     <t>Відрядження</t>
   </si>
   <si>
-    <t>старший солдат</t>
+    <t>вч А0101</t>
+  </si>
+  <si>
+    <t>03.11.2024</t>
+  </si>
+  <si>
+    <t>2024-12-21</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>11.12.2024</t>
+  </si>
+  <si>
+    <t>30.10.2024</t>
   </si>
   <si>
     <t>ГРАБОВА О.І.</t>
   </si>
   <si>
-    <t>вч А0101</t>
-  </si>
-  <si>
-    <t>03.11.2024</t>
-  </si>
-  <si>
-    <t>05.11.2024</t>
-  </si>
-  <si>
-    <t>так</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
     <t>лікарняний</t>
   </si>
   <si>
-    <t>30.10.2024</t>
-  </si>
-  <si>
     <t>02.11.2024</t>
   </si>
   <si>
     <t>ні</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>працівник Збройних Сил України</t>
+  </si>
+  <si>
+    <t>ІВАНОВ Василь Сергійович</t>
+  </si>
+  <si>
+    <t>A1100</t>
   </si>
 </sst>
 </file>
@@ -446,15 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,84 +527,134 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="H2">
-        <v>2418</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>227</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3">
+        <v>230</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3">
-        <v>1123</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3">
-        <v>227</v>
-      </c>
-      <c r="L3">
-        <v>230</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>250</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1 A3:M3 A2:K2 M2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:P3 A4:L4 P4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: changed field types and added data input protection for absence types
</commit_message>
<xml_diff>
--- a/renderer/res/Книга тимчасової відсутності.xlsx
+++ b/renderer/res/Книга тимчасової відсутності.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2DFFF-A438-2A4D-8E42-66F61481704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9BBEA9-62C6-E34E-BD15-3FE6CCE99AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temp_book" sheetId="1" r:id="rId1"/>
+    <sheet name="Типи відсутності" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Номер документу (посвідчення, довідка, направлення, тощо)</t>
   </si>
@@ -91,9 +92,6 @@
     <t>03.11.2024</t>
   </si>
   <si>
-    <t>2024-12-21</t>
-  </si>
-  <si>
     <t>231</t>
   </si>
   <si>
@@ -128,19 +126,48 @@
   </si>
   <si>
     <t>A1100</t>
+  </si>
+  <si>
+    <t>04.01.2025</t>
+  </si>
+  <si>
+    <t>21.12.2024</t>
+  </si>
+  <si>
+    <t>Відпустка основна</t>
+  </si>
+  <si>
+    <t>Лікарняний</t>
+  </si>
+  <si>
+    <t>Стаціонар</t>
+  </si>
+  <si>
+    <t>Відпустка за сімейними обставинами</t>
+  </si>
+  <si>
+    <t>Відпустка за станом здоров'я</t>
+  </si>
+  <si>
+    <t>ВЛК</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,8 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,179 +512,245 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="6" max="16" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1123</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1123</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1">
+        <v>227</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>227</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="1">
+        <v>230</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3">
-        <v>230</v>
-      </c>
-      <c r="P3" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4">
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
         <v>250</v>
       </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>30</v>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:P3 A4:L4 P4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 A3:E4 A2:E2 N2:P2 J2 G1:P1 G3:P4 G2:H2" numberStoredAsText="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Некоректне значення" error="Краще використати одне з значень, вказаних на аркуші &quot;Типи відсутності&quot;" xr:uid="{E9F3366D-8C65-A241-8133-1F4F1BD508B3}">
+          <x14:formula1>
+            <xm:f>'Типи відсутності'!$A$1:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5BE96C-94ED-E14A-B91B-B48A92437A71}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added title index for better compatibility with DR
</commit_message>
<xml_diff>
--- a/renderer/res/Книга тимчасової відсутності.xlsx
+++ b/renderer/res/Книга тимчасової відсутності.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9BBEA9-62C6-E34E-BD15-3FE6CCE99AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1338B9-D7E5-C349-8863-1D99B5F06BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Номер документу (посвідчення, довідка, направлення, тощо)</t>
   </si>
@@ -35,39 +35,42 @@
     <t>Прізвище та ініціали (для наочності)</t>
   </si>
   <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>Тип відсутності</t>
+  </si>
+  <si>
+    <t>Місце тимчасового перебування</t>
+  </si>
+  <si>
+    <t>Дата вибуття</t>
+  </si>
+  <si>
+    <t>Дата наказу, яким вибув</t>
+  </si>
+  <si>
+    <t>Номер наказу, яким вибув</t>
+  </si>
+  <si>
+    <t>Термін відсутності</t>
+  </si>
+  <si>
+    <t>Очікувана дата повернення</t>
+  </si>
+  <si>
+    <t>Реальна дата повернення</t>
+  </si>
+  <si>
+    <t>Дата наказу, яким прибув</t>
+  </si>
+  <si>
+    <t>Номер наказу, яким прибув</t>
+  </si>
+  <si>
     <t>Ідентифікатор військовослужбовця (відповідно до ідентифікатора в словнику)</t>
   </si>
   <si>
-    <t>Тип відсутності</t>
-  </si>
-  <si>
-    <t>Місце тимчасового перебування</t>
-  </si>
-  <si>
-    <t>Дата вибуття</t>
-  </si>
-  <si>
-    <t>Дата наказу, яким вибув</t>
-  </si>
-  <si>
-    <t>Номер наказу, яким вибув</t>
-  </si>
-  <si>
-    <t>Термін відсутності</t>
-  </si>
-  <si>
-    <t>Очікувана дата повернення</t>
-  </si>
-  <si>
-    <t>Реальна дата повернення</t>
-  </si>
-  <si>
-    <t>Дата наказу, яким прибув</t>
-  </si>
-  <si>
-    <t>Номер наказу, яким прибув</t>
-  </si>
-  <si>
     <t>З продовольчим атестатом (так/ні)</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
     <t>ГРАБОВА Олена Ігорівна</t>
   </si>
   <si>
+    <t>0012003</t>
+  </si>
+  <si>
     <t>Відрядження</t>
   </si>
   <si>
@@ -92,55 +98,55 @@
     <t>03.11.2024</t>
   </si>
   <si>
+    <t>21.12.2024</t>
+  </si>
+  <si>
     <t>231</t>
   </si>
   <si>
+    <t>04.01.2025</t>
+  </si>
+  <si>
+    <t>ні</t>
+  </si>
+  <si>
+    <t>30.10.2024</t>
+  </si>
+  <si>
+    <t>ГРАБОВА О.І.</t>
+  </si>
+  <si>
+    <t>лікарняний</t>
+  </si>
+  <si>
+    <t>02.11.2024</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>працівник Збройних Сил України</t>
+  </si>
+  <si>
+    <t>ІВАНОВ Василь Сергійович</t>
+  </si>
+  <si>
+    <t>A1100</t>
+  </si>
+  <si>
     <t>11.12.2024</t>
   </si>
   <si>
-    <t>30.10.2024</t>
-  </si>
-  <si>
-    <t>ГРАБОВА О.І.</t>
-  </si>
-  <si>
-    <t>лікарняний</t>
-  </si>
-  <si>
-    <t>02.11.2024</t>
-  </si>
-  <si>
-    <t>ні</t>
-  </si>
-  <si>
-    <t>221</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>працівник Збройних Сил України</t>
-  </si>
-  <si>
-    <t>ІВАНОВ Василь Сергійович</t>
-  </si>
-  <si>
-    <t>A1100</t>
-  </si>
-  <si>
-    <t>04.01.2025</t>
-  </si>
-  <si>
-    <t>21.12.2024</t>
+    <t>Лікарняний</t>
+  </si>
+  <si>
+    <t>Стаціонар</t>
   </si>
   <si>
     <t>Відпустка основна</t>
-  </si>
-  <si>
-    <t>Лікарняний</t>
-  </si>
-  <si>
-    <t>Стаціонар</t>
   </si>
   <si>
     <t>Відпустка за сімейними обставинами</t>
@@ -156,18 +162,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,11 +191,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,248 +507,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
-    <col min="6" max="16" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3">
+        <v>227</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3">
+        <v>230</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1123</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1">
-        <v>227</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4">
+        <v>250</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>28</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="1">
-        <v>230</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1">
-        <v>250</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A3:E4 A2:E2 N2:P2 J2 G1:P1 G3:P4 G2:H2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:Q1 A3:Q4 A2:L2 P2:Q2" numberStoredAsText="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Некоректне значення" error="Краще використати одне з значень, вказаних на аркуші &quot;Типи відсутності&quot;" xr:uid="{E9F3366D-8C65-A241-8133-1F4F1BD508B3}">
-          <x14:formula1>
-            <xm:f>'Типи відсутності'!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5BE96C-94ED-E14A-B91B-B48A92437A71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
+      <c r="A1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>38</v>
+      <c r="A2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
+      <c r="A3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
+      <c r="A4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
+      <c r="A5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
+      <c r="A6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
+      <c r="A7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:A7" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat:added saving purpose and reason to temp-book
</commit_message>
<xml_diff>
--- a/renderer/res/Книга тимчасової відсутності.xlsx
+++ b/renderer/res/Книга тимчасової відсутності.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB344161-0DAA-AB40-AD46-649F42B1E2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17061775-48F7-064A-AA4A-62BAC0DD6407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Номер документу (посвідчення, довідка, направлення, тощо)</t>
   </si>
@@ -74,6 +74,12 @@
     <t>З продовольчим атестатом (так/ні)</t>
   </si>
   <si>
+    <t>Мета</t>
+  </si>
+  <si>
+    <t>Підстава</t>
+  </si>
+  <si>
     <t>2418</t>
   </si>
   <si>
@@ -104,40 +110,49 @@
     <t>231</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>04.01.2025</t>
   </si>
   <si>
+    <t>04.02.2025</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>ні</t>
   </si>
   <si>
-    <t>30.10.2024</t>
-  </si>
-  <si>
-    <t>ГРАБОВА О.І.</t>
-  </si>
-  <si>
-    <t>лікарняний</t>
-  </si>
-  <si>
-    <t>02.11.2024</t>
-  </si>
-  <si>
-    <t>221</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>05.02.2025</t>
+  </si>
+  <si>
+    <t>працівник Збройних Сил України</t>
+  </si>
+  <si>
+    <t>ІВАНОВ Василь Сергійович</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>працівник Збройних Сил України</t>
-  </si>
-  <si>
-    <t>ІВАНОВ Василь Сергійович</t>
-  </si>
-  <si>
-    <t>A1100</t>
-  </si>
-  <si>
-    <t>11.12.2024</t>
+    <t>військової частини А1111</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>08.02.2025</t>
+  </si>
+  <si>
+    <t>для проведення навчальних стрільб цигарок</t>
+  </si>
+  <si>
+    <t>відсутність гз з 12.01.2025</t>
   </si>
   <si>
     <t>Лікарняний</t>
@@ -507,15 +522,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,131 +582,123 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2">
-        <v>63</v>
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
       </c>
       <c r="P2">
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1123</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3">
-        <v>227</v>
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3">
-        <v>230</v>
+        <v>38</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4">
-        <v>250</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>28</v>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Q4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -706,37 +713,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>